<commit_message>
removed buffer clearing, added initial sql
</commit_message>
<xml_diff>
--- a/student_excel.xlsx
+++ b/student_excel.xlsx
@@ -59,14 +59,6 @@
             <text:p>140536K</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Dileka</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>140660J</text:p>
-          </table:table-cell>
-        </table:table-row>
       </table:table>
       <table:named-expressions/>
     </office:spreadsheet>
@@ -78,11 +70,11 @@
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
   <office:meta>
     <meta:creation-date>2017-03-25T23:13:39.919788644</meta:creation-date>
-    <dc:date>2017-03-25T23:59:08.965626805</dc:date>
-    <meta:editing-duration>PT10M29S</meta:editing-duration>
-    <meta:editing-cycles>4</meta:editing-cycles>
+    <dc:date>2017-04-05T00:27:32.242309260</dc:date>
+    <meta:editing-duration>PT10M56S</meta:editing-duration>
+    <meta:editing-cycles>5</meta:editing-cycles>
     <meta:generator>LibreOffice/5.3.0.3$Linux_X86_64 LibreOffice_project/30m0$Build-3</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="6" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="4" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -94,14 +86,14 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">4515</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">1460</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">973</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">8</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">5</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">15</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -171,7 +163,7 @@
       <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
       <config:config-item config:name="RasterSubdivisionY" config:type="int">1</config:config-item>
       <config:config-item config:name="AutoCalculate" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">rwH+/0Rlc2tqZXQtMTAwMC1KMTEwLXNlcmllcwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAQ1VQUzpEZXNramV0LTEwMDAtSjExMC1zZXJpZXMAAAAWAAMAzAAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9RGVza2pldC0xMDAwLUoxMTAtc2VyaWVzCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpQYWdlU2l6ZTpBNABJbnB1dFNsb3Q6QXV0bwAAEgBDT01QQVRfRFVQTEVYX01PREUTAER1cGxleE1vZGU6OlVua25vd24=</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">rwH+/0Rlc2tqZXQtMTAwMC1KMTEwLXNlcmllcwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAQ1VQUzpEZXNramV0LTEwMDAtSjExMC1zZXJpZXMAAAAWAAMAzAAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9RGVza2pldC0xMDAwLUoxMTAtc2VyaWVzCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpJbnB1dFNsb3Q6QXV0bwBQYWdlU2l6ZTpBNAAAEgBDT01QQVRfRFVQTEVYX01PREUTAER1cGxleE1vZGU6OlVua25vd24=</config:config-item>
       <config:config-item config:name="ApplyUserData" config:type="boolean">true</config:config-item>
       <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
     </config:config-item-set>
@@ -565,9 +557,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2017-03-25">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2017-04-05">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="23:58:22.949088275">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="00:27:06.545992980">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
added contact form mailing
</commit_message>
<xml_diff>
--- a/student_excel.xlsx
+++ b/student_excel.xlsx
@@ -42,21 +42,125 @@
     <office:spreadsheet>
       <table:calculation-settings table:automatic-find-labels="false" table:use-regular-expressions="false" table:use-wildcards="true"/>
       <table:table table:name="Sheet1" table:style-name="ta1">
-        <table:table-column table:style-name="co1" table:number-columns-repeated="2" table:default-cell-style-name="ce1"/>
+        <table:table-column table:style-name="co1" table:number-columns-repeated="2" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>name</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>studentid</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Thejan</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>140536K</text:p>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>thilina</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="170001" calcext:value-type="float">
+            <text:p>170001</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>wishwa</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="170002" calcext:value-type="float">
+            <text:p>170002</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>thathsara</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="170003" calcext:value-type="float">
+            <text:p>170003</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>kisal</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="170004" calcext:value-type="float">
+            <text:p>170004</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>haresha</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="170005" calcext:value-type="float">
+            <text:p>170005</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>chirath</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="170006" calcext:value-type="float">
+            <text:p>170006</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>dinith</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="180001" calcext:value-type="float">
+            <text:p>180001</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>adeesha</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="180002" calcext:value-type="float">
+            <text:p>180002</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>malinthi</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="190001" calcext:value-type="float">
+            <text:p>190001</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>chamodya</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="190002" calcext:value-type="float">
+            <text:p>190002</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>yohan</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="190003" calcext:value-type="float">
+            <text:p>190003</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>uditha</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="190004" calcext:value-type="float">
+            <text:p>190004</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>iduwara</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="190005" calcext:value-type="float">
+            <text:p>190005</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>lasith</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="190006" calcext:value-type="float">
+            <text:p>190006</text:p>
           </table:table-cell>
         </table:table-row>
       </table:table>
@@ -70,11 +174,11 @@
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
   <office:meta>
     <meta:creation-date>2017-03-25T23:13:39.919788644</meta:creation-date>
-    <dc:date>2017-04-05T00:27:32.242309260</dc:date>
-    <meta:editing-duration>PT10M56S</meta:editing-duration>
-    <meta:editing-cycles>5</meta:editing-cycles>
+    <dc:date>2017-04-07T21:41:59.989573296</dc:date>
+    <meta:editing-duration>PT11M23S</meta:editing-duration>
+    <meta:editing-cycles>7</meta:editing-cycles>
     <meta:generator>LibreOffice/5.3.0.3$Linux_X86_64 LibreOffice_project/30m0$Build-3</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="4" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="30" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -86,14 +190,14 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">4515</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">973</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">6808</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">5</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">15</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">6</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -557,9 +661,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2017-04-05">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2017-04-07">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="00:27:06.545992980">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="21:41:42.447908797">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>